<commit_message>
Created forms for my testers
</commit_message>
<xml_diff>
--- a/TimeManagement.xlsx
+++ b/TimeManagement.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,44 +24,106 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Tasks</t>
-  </si>
-  <si>
-    <t>Weeks</t>
-  </si>
-  <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>2 hrs</t>
-  </si>
-  <si>
-    <t>23 hrs</t>
-  </si>
-  <si>
-    <t>9 hrs</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+  <si>
+    <t>Set up a Git Repo</t>
+  </si>
+  <si>
+    <t>Set up Trello for each task</t>
+  </si>
+  <si>
+    <t>Create a sample WPF program</t>
+  </si>
+  <si>
+    <t>Follow online resoure for tips</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasks </t>
+  </si>
+  <si>
+    <t>Task 1 Week 1</t>
+  </si>
+  <si>
+    <t>Task 2 Week 1</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create the methods for URI conn. </t>
+  </si>
+  <si>
+    <t>Figure out how to use oauth 2.0</t>
+  </si>
+  <si>
+    <t>Connect parser and library to sample console</t>
+  </si>
+  <si>
+    <t>Fix bugs that shown up</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3 hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5 hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3  hrs</t>
+  </si>
+  <si>
+    <t>Task 3 : Week 2</t>
+  </si>
+  <si>
+    <t>Connect parser and library to WPF</t>
+  </si>
+  <si>
+    <t>Properly implement library</t>
+  </si>
+  <si>
+    <t>Fix bugs in the from connecting library and  WPf</t>
+  </si>
+  <si>
+    <t>10 hrs</t>
+  </si>
+  <si>
+    <t>5 hrs</t>
+  </si>
+  <si>
+    <t>Task 4: Week 3</t>
+  </si>
+  <si>
+    <t>Write up documentation</t>
+  </si>
+  <si>
+    <t>1 hr</t>
+  </si>
+  <si>
+    <t>Write up log for testers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -90,8 +151,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,57 +434,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A7:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" customWidth="1"/>
+    <col min="2" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="5" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made progress: 4 forms filled, notify function added to capstone_base. No errors as of yet
</commit_message>
<xml_diff>
--- a/TimeManagement.xlsx
+++ b/TimeManagement.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13848"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13848"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Set up a Git Repo</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>Write up log for testers</t>
+  </si>
+  <si>
+    <t>Find up to 10 students to test app</t>
+  </si>
+  <si>
+    <t>Keep a log of suggestions</t>
+  </si>
+  <si>
+    <t>Listen to feedback and make necessary changes</t>
   </si>
 </sst>
 </file>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:B24"/>
+  <dimension ref="A7:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,6 +588,30 @@
         <v>26</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update UI not doing a pdf loader.
</commit_message>
<xml_diff>
--- a/TimeManagement.xlsx
+++ b/TimeManagement.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13848"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13848"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Set up a Git Repo</t>
   </si>
@@ -117,6 +117,33 @@
   </si>
   <si>
     <t>Listen to feedback and make necessary changes</t>
+  </si>
+  <si>
+    <t>Task 5: Week 4</t>
+  </si>
+  <si>
+    <t>Create Icons for notification</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 . 45 hr</t>
+  </si>
+  <si>
+    <t>Make sure application runs from taskbar</t>
+  </si>
+  <si>
+    <t>3 hrs</t>
+  </si>
+  <si>
+    <t>Test notifications</t>
+  </si>
+  <si>
+    <t>Make necessary changes to UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6 hrs</t>
+  </si>
+  <si>
+    <t>6 hrs</t>
   </si>
 </sst>
 </file>
@@ -443,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:B27"/>
+  <dimension ref="A7:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,6 +639,43 @@
         <v>26</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preparing for full ui overhaul
</commit_message>
<xml_diff>
--- a/TimeManagement.xlsx
+++ b/TimeManagement.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Set up a Git Repo</t>
   </si>
@@ -144,6 +144,30 @@
   </si>
   <si>
     <t>6 hrs</t>
+  </si>
+  <si>
+    <t>Task 6 : Week 5</t>
+  </si>
+  <si>
+    <t>10 hr</t>
+  </si>
+  <si>
+    <t>Task 7 : Week 6</t>
+  </si>
+  <si>
+    <t>Research proxy / alert system</t>
+  </si>
+  <si>
+    <t>Set up a alert program</t>
+  </si>
+  <si>
+    <t>Set a timer for alert system</t>
+  </si>
+  <si>
+    <t>19 hrs</t>
+  </si>
+  <si>
+    <t>Task 8: Week 7</t>
   </si>
 </sst>
 </file>
@@ -470,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:B32"/>
+  <dimension ref="A7:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +660,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -674,6 +698,61 @@
       </c>
       <c r="B32" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>